<commit_message>
re-organized IAH207 and PHY410 so exam related material goes into a folder
</commit_message>
<xml_diff>
--- a/CSE232/grade.xlsx
+++ b/CSE232/grade.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispd\classes\SPRING2018\CSE232\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispd\Documents\SPRING2018\CSE232\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F985C1FD-B754-4266-8AA0-F8C9BE731E28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -531,20 +532,20 @@
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="4" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="5" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -557,22 +558,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4">
-        <v>21.84</v>
+        <v>340.35</v>
       </c>
       <c r="E4">
         <v>1000</v>
       </c>
       <c r="G4" s="2">
         <f>D4/E4</f>
-        <v>2.1839999999999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.34035000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -587,7 +588,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -602,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -617,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -632,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -647,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -662,97 +663,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -767,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -788,7 +789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -803,13 +804,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.75">
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.75">
       <c r="D22">
         <f>SUM(D7:D20)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E22">
         <f>SUM(E7:E20)</f>
@@ -817,14 +818,14 @@
       </c>
       <c r="G22">
         <f>D22/E22</f>
-        <v>0.13043478260869565</v>
+        <v>0.39130434782608697</v>
       </c>
       <c r="I22">
         <f>G22*E6</f>
-        <v>6.5217391304347823</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>19.565217391304348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -836,7 +837,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B26" t="s">
         <v>20</v>
       </c>
@@ -851,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -866,97 +867,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>20</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B29" t="s">
         <v>23</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E29">
         <v>30</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B30" t="s">
         <v>24</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>40</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B31" t="s">
         <v>25</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E31">
         <v>50</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.75">
       <c r="B32" t="s">
         <v>26</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E32">
         <v>50</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B33" t="s">
         <v>27</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E33">
         <v>60</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B34" t="s">
         <v>28</v>
       </c>
@@ -971,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B35" t="s">
         <v>29</v>
       </c>
@@ -986,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B36" t="s">
         <v>30</v>
       </c>
@@ -1001,13 +1002,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
       <c r="D38">
         <f>SUM(D26:D36)</f>
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="E38">
         <f>SUM(E26:E36)</f>
@@ -1015,14 +1016,14 @@
       </c>
       <c r="G38">
         <f>D38/E38</f>
-        <v>3.3333333333333333E-2</v>
+        <v>0.56888888888888889</v>
       </c>
       <c r="I38">
         <f>G38*E25</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1034,37 +1035,37 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E42">
         <v>150</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B43" t="s">
         <v>33</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E43">
         <v>150</v>
       </c>
       <c r="G43" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
       <c r="B44" t="s">
         <v>34</v>
       </c>
@@ -1079,13 +1080,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
       <c r="D46">
         <f>SUM(D42:D44)</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="E46">
         <f>SUM(E42:E44)</f>
@@ -1093,14 +1094,14 @@
       </c>
       <c r="G46">
         <f>D46/E46</f>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="I46">
         <f>G46*E41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B50" t="s">
         <v>36</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B51" t="s">
         <v>37</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B52" t="s">
         <v>38</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B53" t="s">
         <v>39</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B54" t="s">
         <v>40</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B55" t="s">
         <v>41</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B56" t="s">
         <v>42</v>
       </c>
@@ -1213,37 +1214,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B57" t="s">
         <v>43</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E57">
         <v>10</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B58" t="s">
         <v>44</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E58">
         <v>10</v>
       </c>
       <c r="G58" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B59" t="s">
         <v>45</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B60" t="s">
         <v>46</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B61" t="s">
         <v>47</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B62" t="s">
         <v>48</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.75">
       <c r="B63" t="s">
         <v>49</v>
       </c>
@@ -1318,13 +1319,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.75">
       <c r="D65">
         <f>SUM(D50:D63)</f>
-        <v>27.78</v>
+        <v>31.71</v>
       </c>
       <c r="E65">
         <f>SUM(E50:E63)</f>
@@ -1332,20 +1333,20 @@
       </c>
       <c r="G65">
         <f>D65/E65</f>
-        <v>0.19842857142857143</v>
+        <v>0.22650000000000001</v>
       </c>
       <c r="I65">
         <f>G65*E49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.75">
       <c r="H69" t="s">
         <v>53</v>
       </c>
       <c r="I69">
         <f>SUM(I22,I38,I46,I65)</f>
-        <v>21.521739130434781</v>
+        <v>515.56521739130437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>